<commit_message>
Avances en notebook y documento
</commit_message>
<xml_diff>
--- a/PRUEBAS HIPOTESIS.xlsx
+++ b/PRUEBAS HIPOTESIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c1858daaa768724f/GITHUB/orange/orange/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6008ECD-57C2-4F55-9AD6-C29634205452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{D6008ECD-57C2-4F55-9AD6-C29634205452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1F1D6A0-697F-4140-AC1F-901442668251}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19965" windowHeight="15600" activeTab="2" xr2:uid="{C100ABFB-0161-41DD-87C4-EFF914B77113}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{C100ABFB-0161-41DD-87C4-EFF914B77113}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>GRUPO</t>
   </si>
@@ -46,15 +46,6 @@
     <t>ESTADÍSTICO</t>
   </si>
   <si>
-    <t>Grande</t>
-  </si>
-  <si>
-    <t>Mediana</t>
-  </si>
-  <si>
-    <t>Pequeña</t>
-  </si>
-  <si>
     <t>P-VALOR</t>
   </si>
   <si>
@@ -64,9 +55,6 @@
     <t>No se rechaza la hipótesis nula. Los datos siguen una distribución normal.</t>
   </si>
   <si>
-    <t>Micro</t>
-  </si>
-  <si>
     <t>ESTADÍSTICO LV</t>
   </si>
   <si>
@@ -77,6 +65,18 @@
   </si>
   <si>
     <t>F-ESTADÍSTICO</t>
+  </si>
+  <si>
+    <t>Manufactura</t>
+  </si>
+  <si>
+    <t>Servicos</t>
+  </si>
+  <si>
+    <t>Comercio</t>
+  </si>
+  <si>
+    <t>Se rechaza la hipótesis nula. Los datos no siguen una distribución normal.</t>
   </si>
 </sst>
 </file>
@@ -155,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -165,10 +165,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -505,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DC3B87-C245-4CE7-8C23-5E7C89DEE9F0}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,88 +523,74 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3">
-        <v>0.91659999999999997</v>
+        <v>0.92259999999999998</v>
       </c>
       <c r="C2" s="3">
-        <v>0.51780000000000004</v>
+        <v>0.2399</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3">
-        <v>0.95609999999999995</v>
+        <v>0.95240000000000002</v>
       </c>
       <c r="C3" s="3">
-        <v>0.62490000000000001</v>
+        <v>0.73550000000000004</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3">
-        <v>0.92949999999999999</v>
+        <v>0.61729999999999996</v>
       </c>
       <c r="C4" s="3">
-        <v>0.59289999999999998</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.96279999999999999</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.79649999999999999</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="A7">
+        <v>0.93669999999999998</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.43830000000000002</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0.93669999999999998</v>
-      </c>
-      <c r="B8" s="5">
-        <v>0.43830000000000002</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -631,24 +614,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0.93669999999999998</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="3">
         <v>0.43830000000000002</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DEAC5C-41C7-4C06-BD93-11D0C4AD0124}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
@@ -673,24 +656,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>12.5298</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="3">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>